<commit_message>
Refactor chemical model and scripts to enhance data handling, update column names, and remove unused code
</commit_message>
<xml_diff>
--- a/assets/file/template/Chemical list section.xlsx
+++ b/assets/file/template/Chemical list section.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\amecnas\amecweb\wwwroot\development\safety\assets\file\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docker\src\safety\assets\file\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E05CC5A-4472-4F7F-9FED-E1EDCC41148B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B81EB3B-A16F-46E8-AD14-4C4B22673ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>LIST OF SEC CHEMICAL SDS REGISTRATION RECORDS</t>
   </si>
@@ -68,46 +68,106 @@
     <t>Class 1</t>
   </si>
   <si>
-    <t>Class 2</t>
-  </si>
-  <si>
-    <t>Class 3</t>
-  </si>
-  <si>
-    <t>Class 4</t>
-  </si>
-  <si>
     <t>Remark : Classification of Hazardous Substances (ประเภทของวัตถุอันตราย)</t>
   </si>
   <si>
-    <t>Explosives   (วัตถุระเบิด)</t>
-  </si>
-  <si>
-    <t>Class 5   Oxidizers and organic peroxides   (ตัวเติมออกซิเจนและสารประกอบอินทรีย์เปอร์ออกไซด์)</t>
-  </si>
-  <si>
-    <t>Gases   (ก๊าซ ต่าง ๆ)</t>
-  </si>
-  <si>
-    <t>Class 6   Poisonous material and Infectious substances (***สารพิษและสารที่ทำให้เกิดโรคติดต่อ***)</t>
-  </si>
-  <si>
-    <t>Flammable Liquid   (ของเหลวไวไฟ)</t>
-  </si>
-  <si>
-    <t>Class 7   Radioactive materials   (สารกัมมันตรังสี)</t>
-  </si>
-  <si>
-    <t>Flammable Solid   (ของแข็งลุกติดไฟได้)</t>
-  </si>
-  <si>
-    <t>Class 8   Corrosive materials   (สารกัดกร่อน)</t>
-  </si>
-  <si>
-    <t>Class 9   Miscellaneous hazardous materials   (สารหรือวัตถุอื่นที่อาจเป็นอันตรายได้)</t>
-  </si>
-  <si>
     <t>Total SDS / SHOP</t>
+  </si>
+  <si>
+    <t>วัตถุระเบิด</t>
+  </si>
+  <si>
+    <t>Class 2A</t>
+  </si>
+  <si>
+    <t>ก๊าซอัด ก๊าซเหลว ก๊าซละลายได้ภายใต้ความดัน</t>
+  </si>
+  <si>
+    <t>Class 2B</t>
+  </si>
+  <si>
+    <t>ก๊าซภายใต้ความดันในกระป๋องเสปร์ย</t>
+  </si>
+  <si>
+    <t>Class 3A</t>
+  </si>
+  <si>
+    <t>ของเหลวไวไฟ จุดวาบไฟไม่เกิน 60 ºC</t>
+  </si>
+  <si>
+    <t>Class 3B</t>
+  </si>
+  <si>
+    <t>ของเหลวไวไฟ จุดวาบไฟมากกว่า 60 ºC-93 ºC คุณสมบัติเข้ากับน้ำไม่ได้</t>
+  </si>
+  <si>
+    <t>Class 4.1A</t>
+  </si>
+  <si>
+    <t>ของแข็งไวไฟ ที่มีคุณสมบัติระเบิด</t>
+  </si>
+  <si>
+    <t>Class 4.1B</t>
+  </si>
+  <si>
+    <t>ของแข็งไวไฟ ที่ไม่มีคุณสมบัติระเบิด</t>
+  </si>
+  <si>
+    <t>Class 4.2</t>
+  </si>
+  <si>
+    <t>สารที่มีความเสี่ยงต่อการลุกไหม้ได้เอง</t>
+  </si>
+  <si>
+    <t>Class 4.3</t>
+  </si>
+  <si>
+    <t>สารให้ก๊าซไวไฟ เมื่อสัมผัสกับน้ำ</t>
+  </si>
+  <si>
+    <t>Class 5.1</t>
+  </si>
+  <si>
+    <t>สารออกซิไดซ์</t>
+  </si>
+  <si>
+    <t>Class 5.2</t>
+  </si>
+  <si>
+    <t>สารเปอร์ออกซิไดซ์</t>
+  </si>
+  <si>
+    <t>Class 6.1A สารติดไฟได้ ที่มีคุณสมบัติเป็นพิษ</t>
+  </si>
+  <si>
+    <t>Class 6.1B สารไม่ติดไฟ ที่มีคุณสมบัติเป็นพิษ</t>
+  </si>
+  <si>
+    <t>Class 6.2 สารติดเชื้อ</t>
+  </si>
+  <si>
+    <t>Class 7 สารกัมมันตรังสี</t>
+  </si>
+  <si>
+    <t>Class 8A สารติดไฟ ที่มีคุณสมบัติกัดกร่อน</t>
+  </si>
+  <si>
+    <t>Class 8B สารไม่ติดไฟ ที่มีคุณสมบัติกัดกร่อน</t>
+  </si>
+  <si>
+    <t>Class 9 วัตถุอันตรายประเภทอื่นๆ</t>
+  </si>
+  <si>
+    <t>Class 10 ของเหลวติดไฟ</t>
+  </si>
+  <si>
+    <t>Class 11 ของแข็งติดไฟได้</t>
+  </si>
+  <si>
+    <t>Class 12 ของเหลวไม่ติดไฟ</t>
+  </si>
+  <si>
+    <t>Class 13 ของแข็งไม่ติดไฟ</t>
   </si>
 </sst>
 </file>
@@ -540,26 +600,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="22.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="22.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="40.7109375" style="1" customWidth="1"/>
-    <col min="8" max="9" width="30.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="40.75" style="1" customWidth="1"/>
+    <col min="8" max="9" width="30.75" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.75" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.375" style="1" customWidth="1"/>
     <col min="13" max="13" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.65">
@@ -631,7 +691,7 @@
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="8" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="11"/>
@@ -642,7 +702,7 @@
     </row>
     <row r="11" spans="1:13" ht="23.25" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="23.25" x14ac:dyDescent="0.5">
@@ -650,48 +710,120 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="23.25" x14ac:dyDescent="0.5">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="23.25" x14ac:dyDescent="0.5">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="23.25" x14ac:dyDescent="0.5">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="23.25" x14ac:dyDescent="0.5">
+      <c r="A16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G16" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="23.25" x14ac:dyDescent="0.5">
+      <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="G16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="23.25" x14ac:dyDescent="0.5">
+      <c r="A18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="23.25" x14ac:dyDescent="0.5">
+      <c r="A19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="23.25" x14ac:dyDescent="0.5">
+      <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="23.25" x14ac:dyDescent="0.5">
+      <c r="A21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="23.25" x14ac:dyDescent="0.5">
+      <c r="A22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>